<commit_message>
Adapting VAT to new structure
</commit_message>
<xml_diff>
--- a/03.Tool/Example_FiscalSim_VAT.xlsx
+++ b/03.Tool/Example_FiscalSim_VAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/dvalderramagonza_worldbank_org/Documents/Example_FiscalSim/03.Tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{CDB0567D-1A59-4F37-9BB8-1D0501BD18FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D2C73BA-7E23-457B-A31C-3DAE6E7460D0}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{CDB0567D-1A59-4F37-9BB8-1D0501BD18FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BF20EBB-9A5C-4247-84F3-2E965CA78FF2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3722" uniqueCount="1484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3723" uniqueCount="1485">
   <si>
     <t>Bracket</t>
   </si>
@@ -4536,7 +4536,10 @@
     <t>no</t>
   </si>
   <si>
-    <t>VAT_exempt_share</t>
+    <t>VAT_exempt_share_SY</t>
+  </si>
+  <si>
+    <t>VAT_exempt_share_PY</t>
   </si>
 </sst>
 </file>
@@ -5788,6 +5791,9 @@
     <xf numFmtId="164" fontId="21" fillId="12" borderId="27" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5868,9 +5874,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -39149,14 +39152,14 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="J44" sqref="J44"/>
       <selection pane="topRight" activeCell="J44" sqref="J44"/>
       <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:W17"/>
+      <selection pane="bottomRight" activeCell="X2" sqref="X2:X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39169,7 +39172,7 @@
     <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1099</v>
       </c>
@@ -39231,16 +39234,19 @@
         <v>1119</v>
       </c>
       <c r="U1" t="s">
+        <v>1483</v>
+      </c>
+      <c r="V1" t="s">
         <v>1101</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>1120</v>
       </c>
-      <c r="W1" t="s">
-        <v>1483</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -39298,18 +39304,23 @@
       <c r="S2" s="129">
         <v>0.18</v>
       </c>
-      <c r="T2" s="195"/>
+      <c r="T2" s="195">
+        <v>0</v>
+      </c>
       <c r="U2" s="129">
-        <f>Parameters!$C$43</f>
-        <v>0.17199999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="V2" s="195">
-        <f>T2</f>
+        <v>0.18</v>
+      </c>
+      <c r="W2" s="243">
         <v>0</v>
       </c>
-      <c r="W2" s="270"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2" s="243">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -39367,18 +39378,19 @@
       <c r="S3" s="129">
         <v>0.25</v>
       </c>
-      <c r="T3" s="195"/>
-      <c r="U3" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="T3" s="195">
+        <v>0</v>
+      </c>
+      <c r="U3" s="129"/>
       <c r="V3" s="195">
-        <f t="shared" ref="V3:V7" si="0">T3</f>
+        <v>0.25</v>
+      </c>
+      <c r="W3" s="243">
         <v>0</v>
       </c>
-      <c r="W3" s="270"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="243"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -39436,18 +39448,19 @@
       <c r="S4" s="129">
         <v>0.25</v>
       </c>
-      <c r="T4" s="195"/>
-      <c r="U4" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="T4" s="195">
+        <v>0</v>
+      </c>
+      <c r="U4" s="129"/>
       <c r="V4" s="195">
-        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W4" s="243">
         <v>0</v>
       </c>
-      <c r="W4" s="270"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="243"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -39505,18 +39518,19 @@
       <c r="S5" s="129">
         <v>0</v>
       </c>
-      <c r="T5" s="195"/>
-      <c r="U5" s="129">
-        <f>Parameters!$C$44</f>
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="T5" s="195">
+        <v>0</v>
+      </c>
+      <c r="U5" s="129"/>
       <c r="V5" s="195">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W5" s="270"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W5" s="243">
+        <v>0</v>
+      </c>
+      <c r="X5" s="243"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -39574,18 +39588,19 @@
       <c r="S6" s="129">
         <v>0.25</v>
       </c>
-      <c r="T6" s="195"/>
-      <c r="U6" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="T6" s="195">
+        <v>0</v>
+      </c>
+      <c r="U6" s="129"/>
       <c r="V6" s="195">
-        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W6" s="243">
         <v>0</v>
       </c>
-      <c r="W6" s="270"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6" s="243"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -39643,18 +39658,19 @@
       <c r="S7" s="129">
         <v>0.25</v>
       </c>
-      <c r="T7" s="195"/>
-      <c r="U7" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="T7" s="195">
+        <v>0</v>
+      </c>
+      <c r="U7" s="129"/>
       <c r="V7" s="195">
-        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="W7" s="243">
         <v>0</v>
       </c>
-      <c r="W7" s="270"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7" s="243"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -39714,17 +39730,17 @@
         <v>1</v>
       </c>
       <c r="U8" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="V8" s="195">
-        <v>0</v>
-      </c>
-      <c r="W8" s="270">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="V8" s="195"/>
+      <c r="W8" s="243">
+        <v>1</v>
+      </c>
+      <c r="X8" s="243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -39782,17 +39798,19 @@
       <c r="S9" s="129">
         <v>0</v>
       </c>
-      <c r="T9" s="195"/>
-      <c r="U9" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="T9" s="195">
+        <v>0</v>
+      </c>
+      <c r="U9" s="129"/>
       <c r="V9" s="195">
         <v>0</v>
       </c>
-      <c r="W9" s="270"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W9" s="243">
+        <v>0</v>
+      </c>
+      <c r="X9" s="243"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -39850,17 +39868,19 @@
       <c r="S10" s="129">
         <v>0.25</v>
       </c>
-      <c r="T10" s="195"/>
-      <c r="U10" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="T10" s="195">
+        <v>0</v>
+      </c>
+      <c r="U10" s="129"/>
       <c r="V10" s="195">
+        <v>0.25</v>
+      </c>
+      <c r="W10" s="243">
         <v>0</v>
       </c>
-      <c r="W10" s="270"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10" s="243"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -39920,17 +39940,19 @@
         <v>1</v>
       </c>
       <c r="U11" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="V11" s="195">
-        <v>0</v>
-      </c>
-      <c r="W11" s="270">
+        <v>0.25</v>
+      </c>
+      <c r="W11" s="243">
+        <v>1</v>
+      </c>
+      <c r="X11" s="243">
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -39990,17 +40012,19 @@
         <v>1</v>
       </c>
       <c r="U12" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="V12" s="195">
-        <v>0</v>
-      </c>
-      <c r="W12" s="270">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="W12" s="243">
+        <v>1</v>
+      </c>
+      <c r="X12" s="243">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -40060,17 +40084,19 @@
         <v>1</v>
       </c>
       <c r="U13" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="V13" s="195">
-        <v>0</v>
-      </c>
-      <c r="W13" s="270">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="W13" s="243">
+        <v>1</v>
+      </c>
+      <c r="X13" s="243">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -40130,17 +40156,19 @@
         <v>1</v>
       </c>
       <c r="U14" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="V14" s="195">
-        <v>0</v>
-      </c>
-      <c r="W14" s="270">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="W14" s="243">
+        <v>1</v>
+      </c>
+      <c r="X14" s="243">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -40200,17 +40228,19 @@
         <v>1</v>
       </c>
       <c r="U15" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="V15" s="195">
-        <v>0</v>
-      </c>
-      <c r="W15" s="270">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="W15" s="243">
+        <v>1</v>
+      </c>
+      <c r="X15" s="243">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -40270,17 +40300,19 @@
         <v>1</v>
       </c>
       <c r="U16" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="V16" s="195">
-        <v>0</v>
-      </c>
-      <c r="W16" s="270">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="W16" s="243">
+        <v>1</v>
+      </c>
+      <c r="X16" s="243">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -40340,14 +40372,16 @@
         <v>1</v>
       </c>
       <c r="U17" s="129">
-        <f>Parameters!$C$42</f>
-        <v>0.17199999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="V17" s="195">
-        <v>0</v>
-      </c>
-      <c r="W17" s="270">
-        <v>0.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="W17" s="243">
+        <v>1</v>
+      </c>
+      <c r="X17" s="243">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -40422,24 +40456,24 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="O3" s="4"/>
-      <c r="Q3" s="243"/>
-      <c r="R3" s="243"/>
-      <c r="S3" s="243"/>
-      <c r="T3" s="243"/>
-      <c r="U3" s="243"/>
-      <c r="V3" s="243"/>
+      <c r="Q3" s="244"/>
+      <c r="R3" s="244"/>
+      <c r="S3" s="244"/>
+      <c r="T3" s="244"/>
+      <c r="U3" s="244"/>
+      <c r="V3" s="244"/>
       <c r="AK3"/>
     </row>
     <row r="4" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
-      <c r="B4" s="244" t="s">
+      <c r="B4" s="245" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="245"/>
-      <c r="D4" s="245"/>
-      <c r="E4" s="245"/>
-      <c r="F4" s="245"/>
-      <c r="G4" s="246"/>
+      <c r="C4" s="246"/>
+      <c r="D4" s="246"/>
+      <c r="E4" s="246"/>
+      <c r="F4" s="246"/>
+      <c r="G4" s="247"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="O4" s="4"/>
@@ -41186,12 +41220,12 @@
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
       <c r="P3" s="4"/>
-      <c r="R3" s="243"/>
-      <c r="S3" s="243"/>
-      <c r="T3" s="243"/>
-      <c r="U3" s="243"/>
-      <c r="V3" s="243"/>
-      <c r="W3" s="243"/>
+      <c r="R3" s="244"/>
+      <c r="S3" s="244"/>
+      <c r="T3" s="244"/>
+      <c r="U3" s="244"/>
+      <c r="V3" s="244"/>
+      <c r="W3" s="244"/>
       <c r="AL3"/>
     </row>
     <row r="4" spans="1:38" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -42219,18 +42253,18 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
-      <c r="X4" s="247" t="s">
+      <c r="X4" s="248" t="s">
         <v>36</v>
       </c>
-      <c r="Y4" s="248"/>
-      <c r="Z4" s="248"/>
-      <c r="AA4" s="248"/>
-      <c r="AB4" s="248"/>
-      <c r="AC4" s="248"/>
-      <c r="AD4" s="248"/>
-      <c r="AE4" s="248"/>
-      <c r="AF4" s="248"/>
-      <c r="AG4" s="249"/>
+      <c r="Y4" s="249"/>
+      <c r="Z4" s="249"/>
+      <c r="AA4" s="249"/>
+      <c r="AB4" s="249"/>
+      <c r="AC4" s="249"/>
+      <c r="AD4" s="249"/>
+      <c r="AE4" s="249"/>
+      <c r="AF4" s="249"/>
+      <c r="AG4" s="250"/>
     </row>
     <row r="5" spans="1:61" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="43"/>
@@ -44273,20 +44307,20 @@
       <c r="B2">
         <v>34626.576694199313</v>
       </c>
-      <c r="E2" s="250" t="s">
+      <c r="E2" s="251" t="s">
         <v>778</v>
       </c>
-      <c r="F2" s="251"/>
-      <c r="G2" s="251"/>
-      <c r="H2" s="251"/>
-      <c r="I2" s="251"/>
-      <c r="J2" s="251"/>
-      <c r="K2" s="251"/>
-      <c r="L2" s="251"/>
-      <c r="M2" s="251"/>
-      <c r="N2" s="251"/>
-      <c r="O2" s="251"/>
-      <c r="P2" s="252"/>
+      <c r="F2" s="252"/>
+      <c r="G2" s="252"/>
+      <c r="H2" s="252"/>
+      <c r="I2" s="252"/>
+      <c r="J2" s="252"/>
+      <c r="K2" s="252"/>
+      <c r="L2" s="252"/>
+      <c r="M2" s="252"/>
+      <c r="N2" s="252"/>
+      <c r="O2" s="252"/>
+      <c r="P2" s="253"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
@@ -44315,10 +44349,10 @@
       <c r="L3" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="253" t="s">
+      <c r="M3" s="254" t="s">
         <v>784</v>
       </c>
-      <c r="N3" s="253"/>
+      <c r="N3" s="254"/>
       <c r="O3" s="113" t="s">
         <v>16</v>
       </c>
@@ -46074,24 +46108,24 @@
   <sheetData>
     <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="4:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="254" t="s">
+      <c r="D5" s="255" t="s">
         <v>795</v>
       </c>
-      <c r="E5" s="255"/>
-      <c r="F5" s="255"/>
-      <c r="G5" s="255"/>
-      <c r="H5" s="256"/>
+      <c r="E5" s="256"/>
+      <c r="F5" s="256"/>
+      <c r="G5" s="256"/>
+      <c r="H5" s="257"/>
     </row>
     <row r="6" spans="4:15" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D6" s="134" t="s">
         <v>796</v>
       </c>
       <c r="E6" s="135"/>
-      <c r="F6" s="257" t="s">
+      <c r="F6" s="258" t="s">
         <v>797</v>
       </c>
-      <c r="G6" s="257"/>
-      <c r="H6" s="258"/>
+      <c r="G6" s="258"/>
+      <c r="H6" s="259"/>
     </row>
     <row r="7" spans="4:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D7" s="136"/>
@@ -46159,21 +46193,21 @@
     </row>
     <row r="13" spans="4:15" ht="13.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="259" t="s">
+      <c r="D14" s="260" t="s">
         <v>803</v>
       </c>
-      <c r="E14" s="260"/>
-      <c r="F14" s="261"/>
-      <c r="H14" s="259" t="s">
+      <c r="E14" s="261"/>
+      <c r="F14" s="262"/>
+      <c r="H14" s="260" t="s">
         <v>804</v>
       </c>
-      <c r="I14" s="260"/>
-      <c r="J14" s="261"/>
-      <c r="M14" s="262" t="s">
+      <c r="I14" s="261"/>
+      <c r="J14" s="262"/>
+      <c r="M14" s="263" t="s">
         <v>805</v>
       </c>
-      <c r="N14" s="263"/>
-      <c r="O14" s="264"/>
+      <c r="N14" s="264"/>
+      <c r="O14" s="265"/>
     </row>
     <row r="15" spans="4:15" s="23" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="130"/>
@@ -46670,13 +46704,13 @@
       <c r="B2" s="168">
         <v>34626.576694199313</v>
       </c>
-      <c r="H2" s="265" t="s">
+      <c r="H2" s="266" t="s">
         <v>1088</v>
       </c>
-      <c r="I2" s="266"/>
-      <c r="J2" s="266"/>
-      <c r="K2" s="266"/>
-      <c r="L2" s="267"/>
+      <c r="I2" s="267"/>
+      <c r="J2" s="267"/>
+      <c r="K2" s="267"/>
+      <c r="L2" s="268"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="168" t="str">
@@ -46690,10 +46724,10 @@
       <c r="J3" s="177" t="s">
         <v>1089</v>
       </c>
-      <c r="K3" s="268" t="s">
+      <c r="K3" s="269" t="s">
         <v>1090</v>
       </c>
-      <c r="L3" s="269"/>
+      <c r="L3" s="270"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="168" t="str">
@@ -48287,6 +48321,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3F2126381553441AAB919CB53585984" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1f1b497080c7a9ebe3361009889ddd89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac8e30ca-65e9-4041-b86a-4d1b6d416c33" xmlns:ns4="fb6f0dd5-0349-47c8-82f6-4423e71a7ac1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a52065183d7b0fe9b0b93a9043295234" ns3:_="" ns4:_="">
     <xsd:import namespace="ac8e30ca-65e9-4041-b86a-4d1b6d416c33"/>
@@ -48509,15 +48552,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -48525,6 +48559,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D121BB-2F17-4CB9-A6EB-F21D520CE0DB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{896EEE12-401D-4484-A123-4E3419FF9B2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -48543,14 +48585,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1D121BB-2F17-4CB9-A6EB-F21D520CE0DB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{688B2FF8-EC2C-43B6-830F-CB3A5682666A}">
   <ds:schemaRefs>

</xml_diff>